<commit_message>
Review Importfiles and other changes
</commit_message>
<xml_diff>
--- a/Test data/TestData.xlsx
+++ b/Test data/TestData.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Seleniumworkspace\Maven_Xcelerate\Test data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="15135" windowHeight="8130" firstSheet="34" activeTab="38"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="15135" windowHeight="8130" firstSheet="27" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="Mercury" sheetId="1" r:id="rId1"/>
@@ -53,7 +48,7 @@
     <sheet name="BankAccountCreation" sheetId="20" r:id="rId39"/>
     <sheet name="ISOPAIN" sheetId="52" r:id="rId40"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -741,9 +736,6 @@
     <t>Test99 - Test099</t>
   </si>
   <si>
-    <t>siri300</t>
-  </si>
-  <si>
     <t>Test5_Entity12</t>
   </si>
   <si>
@@ -759,13 +751,16 @@
     <t>001155</t>
   </si>
   <si>
-    <t>L319</t>
+    <t>L321</t>
+  </si>
+  <si>
+    <t>siri301</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
@@ -1247,7 +1242,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1280,26 +1275,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1332,23 +1310,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8518,8 +8479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8603,7 +8564,7 @@
         <v>80</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>64</v>
@@ -12000,7 +11961,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>82</v>
@@ -12009,7 +11970,7 @@
         <v>84</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>86</v>
@@ -12390,8 +12351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12497,7 +12458,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>213</v>
@@ -12526,7 +12487,7 @@
       </c>
       <c r="M2" s="11" t="str">
         <f>C2</f>
-        <v>L319</v>
+        <v>L321</v>
       </c>
       <c r="N2" s="11">
         <v>1000000</v>
@@ -12542,7 +12503,7 @@
       </c>
       <c r="R2" s="11" t="str">
         <f>C2</f>
-        <v>L319</v>
+        <v>L321</v>
       </c>
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
@@ -13381,16 +13342,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>230</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>231</v>
       </c>
       <c r="E2" s="41" t="s">
         <v>192</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G2" s="20" t="s">
         <v>45</v>
@@ -13399,7 +13360,7 @@
         <v>225</v>
       </c>
       <c r="I2" s="66" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J2" s="20">
         <v>1173782</v>

</xml_diff>

<commit_message>
Bank account creation changes
</commit_message>
<xml_diff>
--- a/Test data/TestData.xlsx
+++ b/Test data/TestData.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1997" uniqueCount="245">
   <si>
     <t>Password</t>
   </si>
@@ -754,7 +754,40 @@
     <t>siri302</t>
   </si>
   <si>
-    <t>L329</t>
+    <t>ServiceId</t>
+  </si>
+  <si>
+    <t>ServiceTypeId</t>
+  </si>
+  <si>
+    <t>ServiceId1</t>
+  </si>
+  <si>
+    <t>ServiceTypeId1</t>
+  </si>
+  <si>
+    <t>Collections</t>
+  </si>
+  <si>
+    <t>Same Day</t>
+  </si>
+  <si>
+    <t>Payments</t>
+  </si>
+  <si>
+    <t>Realtime</t>
+  </si>
+  <si>
+    <t>NAEDO</t>
+  </si>
+  <si>
+    <t>Corp SSV</t>
+  </si>
+  <si>
+    <t>Real-Time gross settlement (payment greater than R5mil)</t>
+  </si>
+  <si>
+    <t>L404</t>
   </si>
 </sst>
 </file>
@@ -8139,7 +8172,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8326,7 +8359,7 @@
         <v>103</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>137</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -8343,7 +8376,7 @@
         <v>103</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>137</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -8360,7 +8393,7 @@
         <v>103</v>
       </c>
       <c r="E4" s="41" t="s">
-        <v>137</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -8377,7 +8410,7 @@
         <v>103</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>137</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -8394,7 +8427,7 @@
         <v>103</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>137</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -8411,7 +8444,7 @@
         <v>103</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>137</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -12352,7 +12385,7 @@
   <dimension ref="A1:AA12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12377,8 +12410,8 @@
     <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="69.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15" customWidth="1"/>
+    <col min="23" max="23" width="17.28515625" customWidth="1"/>
     <col min="24" max="24" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11.140625" bestFit="1" customWidth="1"/>
@@ -12440,10 +12473,18 @@
       <c r="R1" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
+      <c r="S1" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="U1" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="V1" s="14" t="s">
+        <v>236</v>
+      </c>
       <c r="W1" s="14"/>
       <c r="X1" s="14"/>
       <c r="Y1" s="14"/>
@@ -12458,7 +12499,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>213</v>
@@ -12473,10 +12514,10 @@
         <v>30</v>
       </c>
       <c r="H2" s="11">
-        <v>255005</v>
+        <v>1155</v>
       </c>
       <c r="I2" s="11">
-        <v>62239543269</v>
+        <v>1173782</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>212</v>
@@ -12487,7 +12528,7 @@
       </c>
       <c r="M2" s="11" t="str">
         <f>C2</f>
-        <v>L329</v>
+        <v>L404</v>
       </c>
       <c r="N2" s="11">
         <v>1000000</v>
@@ -12503,12 +12544,20 @@
       </c>
       <c r="R2" s="11" t="str">
         <f>C2</f>
-        <v>L329</v>
-      </c>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
+        <v>L404</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>240</v>
+      </c>
       <c r="W2" s="11"/>
       <c r="X2" s="11"/>
       <c r="Y2" s="11"/>
@@ -12535,9 +12584,15 @@
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
+      <c r="T3" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>241</v>
+      </c>
       <c r="W3" s="7"/>
       <c r="X3" s="7"/>
       <c r="Y3" s="7"/>
@@ -12564,9 +12619,13 @@
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
+      <c r="T4" s="7" t="s">
+        <v>240</v>
+      </c>
       <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
+      <c r="V4" s="7" t="s">
+        <v>240</v>
+      </c>
       <c r="W4" s="7"/>
       <c r="X4" s="7"/>
       <c r="Y4" s="7"/>
@@ -12593,9 +12652,13 @@
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
+      <c r="T5" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
+      <c r="V5" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="W5" s="7"/>
       <c r="X5" s="7"/>
       <c r="Y5" s="7"/>
@@ -12622,9 +12685,13 @@
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
+      <c r="T6" s="7" t="s">
+        <v>243</v>
+      </c>
       <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
+      <c r="V6" s="7" t="s">
+        <v>243</v>
+      </c>
       <c r="W6" s="7"/>
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>

</xml_diff>

<commit_message>
BankAccount creation script changes
</commit_message>
<xml_diff>
--- a/Test data/TestData.xlsx
+++ b/Test data/TestData.xlsx
@@ -787,7 +787,7 @@
     <t>Real-Time gross settlement (payment greater than R5mil)</t>
   </si>
   <si>
-    <t>L404</t>
+    <t>L411</t>
   </si>
 </sst>
 </file>
@@ -12385,7 +12385,7 @@
   <dimension ref="A1:AA12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12528,7 +12528,7 @@
       </c>
       <c r="M2" s="11" t="str">
         <f>C2</f>
-        <v>L404</v>
+        <v>L411</v>
       </c>
       <c r="N2" s="11">
         <v>1000000</v>
@@ -12544,7 +12544,7 @@
       </c>
       <c r="R2" s="11" t="str">
         <f>C2</f>
-        <v>L404</v>
+        <v>L411</v>
       </c>
       <c r="S2" s="11" t="s">
         <v>237</v>

</xml_diff>

<commit_message>
NewUser creation changes and updates
</commit_message>
<xml_diff>
--- a/Test data/TestData.xlsx
+++ b/Test data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="15135" windowHeight="8130" firstSheet="25" activeTab="27"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="15135" windowHeight="8130" firstSheet="27" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="Mercury" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2015" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2020" uniqueCount="247">
   <si>
     <t>Password</t>
   </si>
@@ -787,10 +787,13 @@
     <t>L411</t>
   </si>
   <si>
-    <t>Nu22</t>
-  </si>
-  <si>
-    <t>Nu23</t>
+    <t>0843353667</t>
+  </si>
+  <si>
+    <t>Nu51</t>
+  </si>
+  <si>
+    <t>Nu52</t>
   </si>
 </sst>
 </file>
@@ -1118,7 +1121,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1217,6 +1220,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4805,7 +4811,7 @@
   <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4837,13 +4843,13 @@
         <v>0</v>
       </c>
       <c r="F1" s="62" t="s">
-        <v>178</v>
+        <v>223</v>
       </c>
       <c r="G1" s="62" t="s">
         <v>179</v>
       </c>
       <c r="H1" s="62" t="s">
-        <v>223</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -8541,9 +8547,9 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -8558,16 +8564,17 @@
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="70" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="69.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" customWidth="1"/>
+    <col min="16" max="16" width="69.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>33</v>
       </c>
@@ -8595,7 +8602,7 @@
       <c r="I1" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="68" t="s">
         <v>70</v>
       </c>
       <c r="K1" s="14" t="s">
@@ -8610,11 +8617,14 @@
       <c r="N1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="15" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>58</v>
       </c>
@@ -8628,7 +8638,7 @@
         <v>80</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>64</v>
@@ -8642,8 +8652,8 @@
       <c r="I2" s="11">
         <v>112539761</v>
       </c>
-      <c r="J2" s="11">
-        <v>8433543669</v>
+      <c r="J2" s="69" t="s">
+        <v>244</v>
       </c>
       <c r="K2" s="11">
         <v>123697854</v>
@@ -8657,11 +8667,14 @@
       <c r="N2" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>58</v>
       </c>
@@ -8675,7 +8688,7 @@
         <v>80</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>64</v>
@@ -8689,8 +8702,8 @@
       <c r="I3" s="11">
         <v>112539761</v>
       </c>
-      <c r="J3" s="11">
-        <v>8433543669</v>
+      <c r="J3" s="69" t="s">
+        <v>244</v>
       </c>
       <c r="K3" s="11">
         <v>123697854</v>
@@ -8704,11 +8717,14 @@
       <c r="N3" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -8718,14 +8734,15 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="J4" s="66"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="7"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -8735,14 +8752,15 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="J5" s="66"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -8752,14 +8770,15 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="J6" s="66"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" s="7"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -8769,14 +8788,15 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="J7" s="66"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" s="7"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -8786,14 +8806,15 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="J8" s="66"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" s="7"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -8803,14 +8824,15 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="J9" s="66"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9" s="7"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -8820,14 +8842,15 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
+      <c r="J10" s="66"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10" s="7"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -8837,14 +8860,15 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
+      <c r="J11" s="66"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11" s="7"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -8854,16 +8878,21 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
+      <c r="J12" s="66"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O2" r:id="rId1"/>
+    <hyperlink ref="O3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changes pushing on 22-05-19
</commit_message>
<xml_diff>
--- a/Test data/TestData.xlsx
+++ b/Test data/TestData.xlsx
@@ -52,13 +52,14 @@
     <sheet name="B2BSetup" sheetId="55" r:id="rId43"/>
     <sheet name="ACBEbtryClass" sheetId="56" r:id="rId44"/>
     <sheet name="Sheet1" sheetId="57" r:id="rId45"/>
+    <sheet name="Sheet2" sheetId="58" r:id="rId46"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3051" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3065" uniqueCount="421">
   <si>
     <t>Password</t>
   </si>
@@ -1239,9 +1240,6 @@
     <t>User015</t>
   </si>
   <si>
-    <t>2964/214410/01</t>
-  </si>
-  <si>
     <t>Collections Xchange0002</t>
   </si>
   <si>
@@ -1266,7 +1264,64 @@
     <t>No collections adding</t>
   </si>
   <si>
-    <t>NewEntity0065</t>
+    <t>Environment2</t>
+  </si>
+  <si>
+    <t>Xcelerate_SMI-31249</t>
+  </si>
+  <si>
+    <t>ISO QA Description</t>
+  </si>
+  <si>
+    <t>AAb32</t>
+  </si>
+  <si>
+    <t>AAb33</t>
+  </si>
+  <si>
+    <t>25-05-2017</t>
+  </si>
+  <si>
+    <t>2964/214184/20</t>
+  </si>
+  <si>
+    <t>NewEntity021</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>creating batch file</t>
+  </si>
+  <si>
+    <t>Batch processed</t>
+  </si>
+  <si>
+    <t>Batch file created</t>
+  </si>
+  <si>
+    <t>Batch sent</t>
+  </si>
+  <si>
+    <t>op2</t>
+  </si>
+  <si>
+    <t>op3</t>
+  </si>
+  <si>
+    <t>op1</t>
+  </si>
+  <si>
+    <t>op4</t>
+  </si>
+  <si>
+    <t>User022</t>
+  </si>
+  <si>
+    <t>NewEntity022</t>
+  </si>
+  <si>
+    <t>2964/214422/01</t>
   </si>
 </sst>
 </file>
@@ -5596,8 +5651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5610,6 +5665,7 @@
     <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5629,12 +5685,15 @@
         <v>0</v>
       </c>
       <c r="F1" s="59" t="s">
-        <v>176</v>
+        <v>401</v>
       </c>
       <c r="G1" s="59" t="s">
         <v>177</v>
       </c>
       <c r="H1" s="59" t="s">
+        <v>176</v>
+      </c>
+      <c r="I1" s="59" t="s">
         <v>215</v>
       </c>
     </row>
@@ -5663,6 +5722,7 @@
       <c r="H2" s="7" t="s">
         <v>216</v>
       </c>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -5689,6 +5749,7 @@
       <c r="H3" s="7" t="s">
         <v>216</v>
       </c>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -5709,6 +5770,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
       <c r="K4">
         <v>1978</v>
       </c>
@@ -5732,6 +5794,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
       <c r="L5">
         <v>1</v>
       </c>
@@ -5761,6 +5824,7 @@
       <c r="H6" s="7" t="s">
         <v>216</v>
       </c>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -5787,6 +5851,7 @@
       <c r="H7" s="7" t="s">
         <v>216</v>
       </c>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -5811,6 +5876,7 @@
       <c r="H8" s="7" t="s">
         <v>216</v>
       </c>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
@@ -5831,6 +5897,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
@@ -5851,6 +5918,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -5871,6 +5939,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -5891,6 +5960,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -5911,6 +5981,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -5931,6 +6002,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
@@ -5951,6 +6023,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
@@ -5971,8 +6044,9 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>126</v>
       </c>
@@ -5991,8 +6065,9 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>128</v>
       </c>
@@ -6011,8 +6086,9 @@
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>129</v>
       </c>
@@ -6031,8 +6107,9 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>130</v>
       </c>
@@ -6051,8 +6128,9 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>131</v>
       </c>
@@ -6071,8 +6149,9 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>132</v>
       </c>
@@ -6093,8 +6172,9 @@
         <v>200</v>
       </c>
       <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
         <v>137</v>
       </c>
@@ -6113,8 +6193,9 @@
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>337</v>
       </c>
@@ -6139,8 +6220,9 @@
       <c r="H24" s="7" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>201</v>
       </c>
@@ -6165,8 +6247,9 @@
       <c r="H25" s="7" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>293</v>
       </c>
@@ -6191,8 +6274,9 @@
       <c r="H26" s="7" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>292</v>
       </c>
@@ -6215,8 +6299,9 @@
       <c r="H27" s="7" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>336</v>
       </c>
@@ -6235,8 +6320,9 @@
       <c r="F28" s="38"/>
       <c r="G28" s="38"/>
       <c r="H28" s="38"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>338</v>
       </c>
@@ -6255,8 +6341,9 @@
       <c r="F29" s="38"/>
       <c r="G29" s="38"/>
       <c r="H29" s="38"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>347</v>
       </c>
@@ -6279,8 +6366,11 @@
       <c r="H30" s="7" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="7" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>144</v>
       </c>
@@ -6299,8 +6389,9 @@
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>144</v>
       </c>
@@ -6319,6 +6410,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
@@ -6339,6 +6431,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
@@ -6359,6 +6452,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
@@ -6379,6 +6473,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
@@ -6399,6 +6494,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
@@ -6419,6 +6515,7 @@
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
@@ -6439,6 +6536,7 @@
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
@@ -6459,6 +6557,7 @@
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
@@ -6479,6 +6578,7 @@
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
@@ -6499,6 +6599,7 @@
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
@@ -6519,6 +6620,7 @@
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
       <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
@@ -6539,6 +6641,7 @@
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
@@ -6559,6 +6662,7 @@
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
       <c r="K44">
         <v>2017</v>
       </c>
@@ -6585,6 +6689,7 @@
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
       <c r="K45">
         <v>2018</v>
       </c>
@@ -6608,6 +6713,7 @@
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
@@ -6628,6 +6734,7 @@
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
@@ -6648,8 +6755,9 @@
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="7"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>148</v>
       </c>
@@ -6668,8 +6776,9 @@
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="7"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>148</v>
       </c>
@@ -6688,8 +6797,9 @@
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="7"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>147</v>
       </c>
@@ -6708,8 +6818,9 @@
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="7"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>150</v>
       </c>
@@ -6728,8 +6839,9 @@
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="7"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>150</v>
       </c>
@@ -6748,8 +6860,9 @@
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" s="7"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>150</v>
       </c>
@@ -6768,8 +6881,9 @@
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" s="7"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>150</v>
       </c>
@@ -6788,8 +6902,9 @@
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" s="7"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>150</v>
       </c>
@@ -6808,8 +6923,9 @@
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56" s="7"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>150</v>
       </c>
@@ -6828,8 +6944,9 @@
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57" s="7"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>149</v>
       </c>
@@ -6848,8 +6965,9 @@
       <c r="F58" s="7"/>
       <c r="G58" s="7"/>
       <c r="H58" s="7"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" s="7"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>157</v>
       </c>
@@ -6868,8 +6986,9 @@
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" s="7"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>157</v>
       </c>
@@ -6888,8 +7007,9 @@
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" s="7"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>157</v>
       </c>
@@ -6908,8 +7028,9 @@
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" s="7"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>157</v>
       </c>
@@ -6928,8 +7049,9 @@
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" s="7"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>157</v>
       </c>
@@ -6948,8 +7070,9 @@
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" s="7"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>157</v>
       </c>
@@ -6968,8 +7091,9 @@
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64" s="7"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>156</v>
       </c>
@@ -6988,8 +7112,9 @@
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65" s="7"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>155</v>
       </c>
@@ -7008,8 +7133,9 @@
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
       <c r="H66" s="7"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" s="7"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>155</v>
       </c>
@@ -7028,8 +7154,9 @@
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
       <c r="H67" s="7"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67" s="7"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>155</v>
       </c>
@@ -7048,8 +7175,9 @@
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" s="7"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>155</v>
       </c>
@@ -7068,8 +7196,9 @@
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69" s="7"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>155</v>
       </c>
@@ -7088,8 +7217,9 @@
       <c r="F70" s="7"/>
       <c r="G70" s="7"/>
       <c r="H70" s="7"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" s="7"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>155</v>
       </c>
@@ -7108,8 +7238,9 @@
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
       <c r="H71" s="7"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" s="7"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>154</v>
       </c>
@@ -7128,8 +7259,9 @@
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
       <c r="H72" s="7"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" s="7"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>165</v>
       </c>
@@ -7148,8 +7280,9 @@
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
       <c r="H73" s="7"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="7"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>165</v>
       </c>
@@ -7168,8 +7301,9 @@
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
       <c r="H74" s="7"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74" s="7"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>165</v>
       </c>
@@ -7188,8 +7322,9 @@
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
       <c r="H75" s="7"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" s="7"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>165</v>
       </c>
@@ -7208,8 +7343,9 @@
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
       <c r="H76" s="7"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" s="7"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>165</v>
       </c>
@@ -7228,8 +7364,9 @@
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
       <c r="H77" s="7"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" s="7"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>165</v>
       </c>
@@ -7248,8 +7385,9 @@
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
       <c r="H78" s="7"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="7"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>164</v>
       </c>
@@ -7268,8 +7406,9 @@
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
       <c r="H79" s="7"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" s="7"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>163</v>
       </c>
@@ -7288,8 +7427,9 @@
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
       <c r="H80" s="7"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="7"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>163</v>
       </c>
@@ -7308,8 +7448,9 @@
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
       <c r="H81" s="7"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="7"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>163</v>
       </c>
@@ -7328,8 +7469,9 @@
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
       <c r="H82" s="7"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" s="7"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>163</v>
       </c>
@@ -7348,8 +7490,9 @@
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
       <c r="H83" s="7"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" s="7"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>163</v>
       </c>
@@ -7368,8 +7511,9 @@
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
       <c r="H84" s="7"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" s="7"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>163</v>
       </c>
@@ -7388,8 +7532,9 @@
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
       <c r="H85" s="7"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" s="7"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>162</v>
       </c>
@@ -7408,8 +7553,9 @@
       <c r="F86" s="7"/>
       <c r="G86" s="7"/>
       <c r="H86" s="7"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" s="7"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>161</v>
       </c>
@@ -7428,8 +7574,9 @@
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
       <c r="H87" s="7"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" s="7"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>161</v>
       </c>
@@ -7448,8 +7595,9 @@
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
       <c r="H88" s="7"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" s="7"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>161</v>
       </c>
@@ -7468,8 +7616,9 @@
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
       <c r="H89" s="7"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89" s="7"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>161</v>
       </c>
@@ -7488,8 +7637,9 @@
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
       <c r="H90" s="7"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" s="7"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>161</v>
       </c>
@@ -7508,8 +7658,9 @@
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
       <c r="H91" s="7"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" s="7"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>161</v>
       </c>
@@ -7528,8 +7679,9 @@
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
       <c r="H92" s="7"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" s="7"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>160</v>
       </c>
@@ -7548,8 +7700,9 @@
       <c r="F93" s="7"/>
       <c r="G93" s="7"/>
       <c r="H93" s="7"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" s="7"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>159</v>
       </c>
@@ -7568,8 +7721,9 @@
       <c r="F94" s="7"/>
       <c r="G94" s="7"/>
       <c r="H94" s="7"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" s="7"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>159</v>
       </c>
@@ -7588,8 +7742,9 @@
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
       <c r="H95" s="7"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95" s="7"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>159</v>
       </c>
@@ -7608,8 +7763,9 @@
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
       <c r="H96" s="7"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96" s="7"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>159</v>
       </c>
@@ -7628,8 +7784,9 @@
       <c r="F97" s="7"/>
       <c r="G97" s="7"/>
       <c r="H97" s="7"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97" s="7"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>159</v>
       </c>
@@ -7648,8 +7805,9 @@
       <c r="F98" s="7"/>
       <c r="G98" s="7"/>
       <c r="H98" s="7"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98" s="7"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>159</v>
       </c>
@@ -7668,8 +7826,9 @@
       <c r="F99" s="7"/>
       <c r="G99" s="7"/>
       <c r="H99" s="7"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99" s="7"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>158</v>
       </c>
@@ -7688,8 +7847,9 @@
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
       <c r="H100" s="7"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I100" s="7"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
         <v>153</v>
       </c>
@@ -7708,8 +7868,9 @@
       <c r="F101" s="7"/>
       <c r="G101" s="7"/>
       <c r="H101" s="7"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101" s="7"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
         <v>153</v>
       </c>
@@ -7728,8 +7889,9 @@
       <c r="F102" s="7"/>
       <c r="G102" s="7"/>
       <c r="H102" s="7"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I102" s="7"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>153</v>
       </c>
@@ -7748,8 +7910,9 @@
       <c r="F103" s="7"/>
       <c r="G103" s="7"/>
       <c r="H103" s="7"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I103" s="7"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
         <v>153</v>
       </c>
@@ -7768,8 +7931,9 @@
       <c r="F104" s="7"/>
       <c r="G104" s="7"/>
       <c r="H104" s="7"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I104" s="7"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>153</v>
       </c>
@@ -7788,8 +7952,9 @@
       <c r="F105" s="7"/>
       <c r="G105" s="7"/>
       <c r="H105" s="7"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I105" s="7"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>153</v>
       </c>
@@ -7808,8 +7973,9 @@
       <c r="F106" s="7"/>
       <c r="G106" s="7"/>
       <c r="H106" s="7"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I106" s="7"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>152</v>
       </c>
@@ -7828,8 +7994,9 @@
       <c r="F107" s="7"/>
       <c r="G107" s="7"/>
       <c r="H107" s="7"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I107" s="7"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="38" t="s">
         <v>189</v>
       </c>
@@ -7854,8 +8021,9 @@
       <c r="H108" s="7" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I108" s="7"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
         <v>233</v>
       </c>
@@ -7878,8 +8046,9 @@
       <c r="H109" s="7" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I109" s="7"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>233</v>
       </c>
@@ -7902,6 +8071,7 @@
       <c r="H110" s="7" t="s">
         <v>216</v>
       </c>
+      <c r="I110" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -13643,8 +13813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14998,8 +15168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DH35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15091,6 +15261,7 @@
     <col min="96" max="96" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="100" max="100" width="17" bestFit="1" customWidth="1"/>
     <col min="104" max="104" width="14.5703125" customWidth="1"/>
+    <col min="106" max="106" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:112" s="99" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -15445,7 +15616,7 @@
         <v>80</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>341</v>
+        <v>405</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>64</v>
@@ -15669,7 +15840,7 @@
         <v>80</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>342</v>
+        <v>404</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>64</v>
@@ -16007,9 +16178,14 @@
       <c r="CR4" s="7"/>
     </row>
     <row r="5" spans="1:112" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:112" x14ac:dyDescent="0.25">
+      <c r="Q6" s="52" t="s">
+        <v>408</v>
+      </c>
+    </row>
     <row r="7" spans="1:112" x14ac:dyDescent="0.25">
       <c r="Q7" s="52" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="8" spans="1:112" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16062,7 +16238,7 @@
         <v>78</v>
       </c>
       <c r="Q8" s="52" t="s">
-        <v>402</v>
+        <v>419</v>
       </c>
       <c r="R8" s="7" t="s">
         <v>82</v>
@@ -16071,7 +16247,7 @@
         <v>84</v>
       </c>
       <c r="T8" s="52" t="s">
-        <v>393</v>
+        <v>420</v>
       </c>
       <c r="U8" s="7" t="s">
         <v>86</v>
@@ -16145,14 +16321,14 @@
       <c r="AR8" s="51" t="s">
         <v>247</v>
       </c>
-      <c r="AS8" s="38" t="s">
-        <v>249</v>
-      </c>
-      <c r="AT8" s="7">
-        <v>62239543269</v>
-      </c>
-      <c r="AU8" s="7" t="s">
-        <v>108</v>
+      <c r="AS8" s="99" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT8" s="99">
+        <v>62006676772</v>
+      </c>
+      <c r="AU8" s="99" t="s">
+        <v>403</v>
       </c>
       <c r="AV8" s="39" t="s">
         <v>250</v>
@@ -16213,7 +16389,7 @@
         <v>190</v>
       </c>
       <c r="CV8" s="52" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="CW8" s="7" t="s">
         <v>386</v>
@@ -16230,8 +16406,8 @@
       <c r="DA8" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="DB8" s="39" t="s">
-        <v>217</v>
+      <c r="DB8" s="99" t="s">
+        <v>403</v>
       </c>
       <c r="DC8">
         <v>16445</v>
@@ -16311,7 +16487,7 @@
         <v>84</v>
       </c>
       <c r="T9" s="11" t="s">
-        <v>346</v>
+        <v>407</v>
       </c>
       <c r="U9" s="11" t="s">
         <v>86</v>
@@ -16691,7 +16867,7 @@
         <v>80</v>
       </c>
       <c r="E11" s="107" t="s">
-        <v>392</v>
+        <v>418</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>348</v>
@@ -16950,10 +17126,10 @@
         <v>371</v>
       </c>
       <c r="CK11" s="19" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="CL11" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="CM11" s="11" t="s">
         <v>225</v>
@@ -16968,7 +17144,7 @@
         <v>331</v>
       </c>
       <c r="CQ11" s="106" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="CR11" s="5" t="s">
         <v>390</v>
@@ -17097,10 +17273,10 @@
         <v>372</v>
       </c>
       <c r="CK12" s="19" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="CL12" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="CM12" s="11" t="s">
         <v>225</v>
@@ -17115,7 +17291,7 @@
         <v>330</v>
       </c>
       <c r="CQ12" s="106" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="CR12" s="7"/>
       <c r="CS12" s="7"/>
@@ -17282,6 +17458,9 @@
       <c r="DH13" s="7"/>
     </row>
     <row r="14" spans="1:112" x14ac:dyDescent="0.25">
+      <c r="E14" s="107" t="s">
+        <v>392</v>
+      </c>
       <c r="BL14" s="42"/>
       <c r="BM14" s="42"/>
       <c r="BN14" s="42"/>
@@ -17332,9 +17511,12 @@
       <c r="A20" s="42"/>
       <c r="B20" s="42"/>
       <c r="CL20" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="CW20" s="99"/>
+      <c r="CZ20" t="s">
+        <v>409</v>
+      </c>
     </row>
     <row r="21" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A21" s="42"/>
@@ -17350,6 +17532,9 @@
       <c r="CN21">
         <v>10.029999999999999</v>
       </c>
+      <c r="CZ21" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="22" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A22" s="42"/>
@@ -17365,6 +17550,9 @@
       </c>
       <c r="CR22" s="99"/>
       <c r="CW22" s="99"/>
+      <c r="CZ22" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="23" spans="1:106" x14ac:dyDescent="0.25">
       <c r="CL23">
@@ -17375,6 +17563,9 @@
       </c>
       <c r="CU23" s="99"/>
       <c r="CY23" s="99"/>
+      <c r="CZ23" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="24" spans="1:106" x14ac:dyDescent="0.25">
       <c r="CJ24">
@@ -17386,6 +17577,9 @@
       </c>
       <c r="CN24">
         <v>10.039999999999999</v>
+      </c>
+      <c r="CZ24" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="25" spans="1:106" x14ac:dyDescent="0.25">
@@ -18351,7 +18545,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:J2"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18508,10 +18702,10 @@
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CQ4"/>
+  <dimension ref="A1:CQ22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD4"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19375,6 +19569,63 @@
       <c r="CP4" s="7"/>
       <c r="CQ4" s="7"/>
     </row>
+    <row r="18" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>2338.69</v>
+      </c>
+      <c r="N18">
+        <v>3095</v>
+      </c>
+    </row>
+    <row r="19" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>416</v>
+      </c>
+      <c r="G19">
+        <f>3*5725.5</f>
+        <v>17176.5</v>
+      </c>
+      <c r="N19">
+        <v>29666</v>
+      </c>
+      <c r="O19">
+        <v>-2419</v>
+      </c>
+    </row>
+    <row r="20" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>414</v>
+      </c>
+      <c r="G20">
+        <f>4294.13*3+16*242.9</f>
+        <v>16768.79</v>
+      </c>
+      <c r="N20">
+        <v>872000</v>
+      </c>
+    </row>
+    <row r="21" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>415</v>
+      </c>
+      <c r="G21">
+        <f>3339.88*3+16*477.13</f>
+        <v>17653.72</v>
+      </c>
+      <c r="I21">
+        <f>17176.5-16768.79</f>
+        <v>407.70999999999913</v>
+      </c>
+    </row>
+    <row r="22" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>417</v>
+      </c>
+      <c r="G22">
+        <f>1431.38*12</f>
+        <v>17176.560000000001</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1"/>
@@ -19382,6 +19633,288 @@
     <hyperlink ref="S2" r:id="rId3" display="P@ssw0rd"/>
     <hyperlink ref="S3" r:id="rId4" display="P@ssw0rd"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F4:I27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>406</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>9</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>11</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="I10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>9</v>
+      </c>
+      <c r="I12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>11</v>
+      </c>
+      <c r="I14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>12</v>
+      </c>
+      <c r="I15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>13</v>
+      </c>
+      <c r="I16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <v>14</v>
+      </c>
+      <c r="I17">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>7</v>
+      </c>
+      <c r="G18">
+        <v>15</v>
+      </c>
+      <c r="I18">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>16</v>
+      </c>
+      <c r="I19">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>9</v>
+      </c>
+      <c r="G20">
+        <v>17</v>
+      </c>
+      <c r="I20">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="G21">
+        <v>18</v>
+      </c>
+      <c r="I21">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>11</v>
+      </c>
+      <c r="G22">
+        <v>19</v>
+      </c>
+      <c r="I22">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>12</v>
+      </c>
+      <c r="G23">
+        <v>20</v>
+      </c>
+      <c r="I23">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>21</v>
+      </c>
+      <c r="I24">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>22</v>
+      </c>
+      <c r="I25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>23</v>
+      </c>
+      <c r="I26">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <v>24</v>
+      </c>
+      <c r="I27">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Commit date on 7-9-21
</commit_message>
<xml_diff>
--- a/Test data/TestData.xlsx
+++ b/Test data/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srinir.SOLARSYSTEM\Desktop\Seleniumworkspace\Xcelerate_Maven\Test data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://qsurehosting-my.sharepoint.com/personal/srinir_qsure_co_za/Documents/Desktop/New folder (2)/Seleniumworkspace/Xcelerate_Maven/Test data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84910530-4DDC-43C2-A28A-C3D3AF8E2876}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{84910530-4DDC-43C2-A28A-C3D3AF8E2876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1330FB6-C273-42DD-A9E9-067756FF863B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1329,9 +1329,6 @@
     <t>2968/211111/98</t>
   </si>
   <si>
-    <t>Xcelerate</t>
-  </si>
-  <si>
     <t>2020-03-01 TO 2020-04-15</t>
   </si>
   <si>
@@ -1377,13 +1374,16 @@
     <t>ambledown financial services</t>
   </si>
   <si>
-    <t>User258</t>
-  </si>
-  <si>
-    <t>NewEntity258</t>
-  </si>
-  <si>
-    <t>2964/214258/21</t>
+    <t>NewEntity259</t>
+  </si>
+  <si>
+    <t>2964/214259/21</t>
+  </si>
+  <si>
+    <t>Xcelerate_PROD</t>
+  </si>
+  <si>
+    <t>User261</t>
   </si>
 </sst>
 </file>
@@ -6135,7 +6135,7 @@
   <dimension ref="A1:M126"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6169,28 +6169,28 @@
         <v>0</v>
       </c>
       <c r="F1" s="59" t="s">
-        <v>176</v>
+        <v>215</v>
       </c>
       <c r="G1" s="59" t="s">
         <v>177</v>
       </c>
       <c r="H1" s="59" t="s">
-        <v>215</v>
+        <v>176</v>
       </c>
       <c r="I1" s="59" t="s">
         <v>395</v>
       </c>
       <c r="J1" s="59" t="s">
+        <v>420</v>
+      </c>
+      <c r="K1" s="110" t="s">
         <v>421</v>
       </c>
-      <c r="K1" s="110" t="s">
-        <v>422</v>
-      </c>
       <c r="L1" s="110" t="s">
+        <v>423</v>
+      </c>
+      <c r="M1" s="110" t="s">
         <v>424</v>
-      </c>
-      <c r="M1" s="110" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -6216,7 +6216,7 @@
         <v>42</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="I2" s="7"/>
     </row>
@@ -6243,7 +6243,7 @@
         <v>178</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="I3" s="7"/>
     </row>
@@ -6312,7 +6312,7 @@
         <v>179</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="I6" s="7"/>
     </row>
@@ -6339,7 +6339,7 @@
         <v>179</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="I7" s="7"/>
     </row>
@@ -6364,7 +6364,7 @@
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="I8" s="7"/>
     </row>
@@ -6408,7 +6408,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="I10" s="7"/>
     </row>
@@ -6710,7 +6710,7 @@
         <v>179</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="I24" s="7"/>
     </row>
@@ -6737,7 +6737,7 @@
         <v>179</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="I25" s="7"/>
     </row>
@@ -6764,7 +6764,7 @@
         <v>178</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="I26" s="7"/>
     </row>
@@ -6789,7 +6789,7 @@
       </c>
       <c r="G27" s="38"/>
       <c r="H27" s="7" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="I27" s="7"/>
     </row>
@@ -6846,7 +6846,7 @@
         <v>180</v>
       </c>
       <c r="D30" s="91" t="s">
-        <v>202</v>
+        <v>133</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>16</v>
@@ -6856,19 +6856,19 @@
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="7" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="I30" s="7" t="s">
         <v>396</v>
       </c>
       <c r="J30" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="K30" t="s">
+        <v>422</v>
+      </c>
+      <c r="L30" t="s">
         <v>426</v>
-      </c>
-      <c r="K30" t="s">
-        <v>423</v>
-      </c>
-      <c r="L30" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -8511,7 +8511,7 @@
         <v>179</v>
       </c>
       <c r="H108" s="7" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="I108" s="7"/>
     </row>
@@ -8536,7 +8536,7 @@
       </c>
       <c r="G109" s="7"/>
       <c r="H109" s="7" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="I109" s="7"/>
     </row>
@@ -8561,7 +8561,7 @@
       </c>
       <c r="G110" s="7"/>
       <c r="H110" s="7" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="I110" s="7"/>
     </row>
@@ -10626,8 +10626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:GV53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11071,7 +11071,7 @@
         <v>112</v>
       </c>
       <c r="DL1" s="17" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="DM1" s="18" t="s">
         <v>114</v>
@@ -11667,10 +11667,10 @@
         <v>402</v>
       </c>
       <c r="Q7" s="52" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="R7" s="52" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="8" spans="1:204" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11723,7 +11723,7 @@
         <v>78</v>
       </c>
       <c r="Q8" s="52" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="R8" s="7" t="s">
         <v>82</v>
@@ -11732,7 +11732,7 @@
         <v>84</v>
       </c>
       <c r="T8" s="52" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="U8" s="7" t="s">
         <v>86</v>
@@ -11919,7 +11919,7 @@
         <v>116</v>
       </c>
       <c r="DK8" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="DL8" s="21">
         <v>201</v>
@@ -12284,7 +12284,7 @@
         <v>116</v>
       </c>
       <c r="DK9" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="DL9" s="21">
         <v>300</v>
@@ -12461,7 +12461,7 @@
         <v>116</v>
       </c>
       <c r="DK10" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="DL10" s="21">
         <v>200</v>
@@ -12484,7 +12484,7 @@
         <v>80</v>
       </c>
       <c r="E11" s="107" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>342</v>
@@ -12796,7 +12796,7 @@
         <v>116</v>
       </c>
       <c r="DK11" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="DL11" s="21">
         <v>3</v>
@@ -12955,7 +12955,7 @@
         <v>116</v>
       </c>
       <c r="DK12" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="DL12" s="21">
         <v>200</v>
@@ -13114,7 +13114,7 @@
         <v>116</v>
       </c>
       <c r="DK13" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="DL13" s="21">
         <v>300</v>
@@ -15183,7 +15183,7 @@
         <v>315</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H2" s="19">
         <v>201</v>
@@ -15192,7 +15192,7 @@
         <v>116</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K2" s="19">
         <v>201</v>
@@ -15221,7 +15221,7 @@
         <v>305</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H3" s="21">
         <v>300</v>
@@ -15230,7 +15230,7 @@
         <v>116</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K3" s="21">
         <v>300</v>
@@ -15259,7 +15259,7 @@
         <v>310</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H4" s="19">
         <v>200</v>
@@ -15268,7 +15268,7 @@
         <v>116</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K4" s="19">
         <v>200</v>
@@ -15297,7 +15297,7 @@
         <v>311</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H5" s="21">
         <v>300</v>
@@ -15306,7 +15306,7 @@
         <v>116</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K5" s="21">
         <v>300</v>
@@ -15335,7 +15335,7 @@
         <v>307</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H6" s="19">
         <v>200</v>
@@ -15344,7 +15344,7 @@
         <v>116</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K6" s="19">
         <v>200</v>
@@ -15373,7 +15373,7 @@
         <v>308</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H7" s="21">
         <v>300</v>
@@ -15382,7 +15382,7 @@
         <v>116</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K7" s="21">
         <v>300</v>
@@ -15399,7 +15399,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
@@ -17110,7 +17110,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>211</v>

</xml_diff>